<commit_message>
typo in alcr distance (20.5, not 70.5)
</commit_message>
<xml_diff>
--- a/data/distances/Dalton_spp_distance_2021_raw.xlsx
+++ b/data/distances/Dalton_spp_distance_2021_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinehayes/Google Drive/Projects/Reburns/Chapters/Flammabllity/data/dispersal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinehayes/Google Drive/Projects/Reburns/Chapters/Flammabllity/data/distances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA1A582-1696-AE4D-B3BB-E98429FF51CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6E0557-8ED0-4A49-B838-8FE55252385D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16480" xr2:uid="{5CB5EA5D-90A9-6B48-9766-250200053600}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{5CB5EA5D-90A9-6B48-9766-250200053600}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A23B7D3A-7E88-CB41-9E7B-E5294CBBCD25}">
   <dimension ref="A1:H876"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A839" zoomScale="88" workbookViewId="0">
-      <selection activeCell="F832" sqref="F832"/>
+    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="88" workbookViewId="0">
+      <selection activeCell="F437" sqref="F437"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10548,8 +10548,8 @@
       <c r="E436" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G436">
-        <v>70.5</v>
+      <c r="F436">
+        <v>20.5</v>
       </c>
       <c r="H436" t="s">
         <v>14</v>

</xml_diff>